<commit_message>
add edit employee-code logic
</commit_message>
<xml_diff>
--- a/temp-peyroll-form/Overall-payroll.xlsx
+++ b/temp-peyroll-form/Overall-payroll.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Congty\thienphumut\test\temp-peyroll-form\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Congty\thienphumut\test\thienphumut-hr-backend\temp-peyroll-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{584E05BC-4C84-4090-B2A2-548E9183D237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C51A0CA-584A-4B74-B552-5D8F32EEBEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{D457F286-B932-415A-9CBA-56FD1E6E92B6}"/>
+    <workbookView xWindow="13577" yWindow="3266" windowWidth="16457" windowHeight="9454" xr2:uid="{D457F286-B932-415A-9CBA-56FD1E6E92B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,9 +99,6 @@
     <t>VND 40,000</t>
   </si>
   <si>
-    <t>Nguyễn Văn A</t>
-  </si>
-  <si>
     <t>Kế toán</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>01117</t>
+  </si>
+  <si>
+    <t>Đoàn Đăng</t>
   </si>
 </sst>
 </file>
@@ -185,7 +185,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$VND]\ #,##0"/>
+    <numFmt numFmtId="164" formatCode="[$VND]\ #,##0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -248,14 +248,14 @@
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -285,7 +285,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -606,7 +606,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -794,120 +794,120 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="F5" s="3">
         <v>6530734221</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="3">
         <v>26</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="3">
         <v>3</v>
       </c>
       <c r="K5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="Q5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="S5" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="D6" s="6">
         <v>45665</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="3">
         <v>6539434276</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="3">
         <v>24</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J6" s="3">
         <v>1.5</v>
       </c>
       <c r="K6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="Q6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="S6" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Update: mail transfer format
</commit_message>
<xml_diff>
--- a/temp-peyroll-form/Overall-payroll.xlsx
+++ b/temp-peyroll-form/Overall-payroll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Congty\thienphumut\test\thienphumut-hr-backend\temp-peyroll-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C51A0CA-584A-4B74-B552-5D8F32EEBEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B495A0DD-5E7E-47BA-BC5E-9C35EE0C64B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13577" yWindow="3266" windowWidth="16457" windowHeight="9454" xr2:uid="{D457F286-B932-415A-9CBA-56FD1E6E92B6}"/>
+    <workbookView xWindow="-10910" yWindow="-110" windowWidth="11020" windowHeight="18700" xr2:uid="{D457F286-B932-415A-9CBA-56FD1E6E92B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="117">
   <si>
     <t>Mã NV</t>
   </si>
@@ -138,9 +138,6 @@
     <t>VND 8,856,500</t>
   </si>
   <si>
-    <t>Đoàn Văn B</t>
-  </si>
-  <si>
     <t>Nhân sự</t>
   </si>
   <si>
@@ -177,7 +174,208 @@
     <t>01117</t>
   </si>
   <si>
-    <t>Đoàn Đăng</t>
+    <t>Số ngày lễ</t>
+  </si>
+  <si>
+    <t>Tiền lễ</t>
+  </si>
+  <si>
+    <t>Số ngày công nghỉ phép/kết hôn/TNLĐ</t>
+  </si>
+  <si>
+    <t>Tiền ngày công nghỉ phép/kết hôn/TNLĐ</t>
+  </si>
+  <si>
+    <t>Phụ cấp trách nhiệm</t>
+  </si>
+  <si>
+    <t>Phụ cấp độc hại</t>
+  </si>
+  <si>
+    <t>Phụ cấp thâm niên</t>
+  </si>
+  <si>
+    <t>Số ngày Tăng ca ngày thường 200%</t>
+  </si>
+  <si>
+    <t>Tiền tăng ca ngày thường 200%</t>
+  </si>
+  <si>
+    <t>Số ngày tăng ca ngày thường 300%</t>
+  </si>
+  <si>
+    <t>Tiền tăng ca ngày thường 300%</t>
+  </si>
+  <si>
+    <t>Số ngày chuyên cần</t>
+  </si>
+  <si>
+    <t>Tiền chuyên cần</t>
+  </si>
+  <si>
+    <t>Số ngày bù lương</t>
+  </si>
+  <si>
+    <t>Tiền bù lương</t>
+  </si>
+  <si>
+    <t>Tiền thưởng sáng kiến</t>
+  </si>
+  <si>
+    <t>Số ngày hỗ trợ đám hiếu/ hỷ</t>
+  </si>
+  <si>
+    <t>Tiền hỗ trợ đám hiếu/ hỷ</t>
+  </si>
+  <si>
+    <t>Số ngày phép năm đã sử dụng</t>
+  </si>
+  <si>
+    <t>Tiền ngày phép năm đã sử dụng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Số ngày phép năm còn lại </t>
+  </si>
+  <si>
+    <t>Tiền thưởng tháng 13</t>
+  </si>
+  <si>
+    <t>Trợ cấp đội trưởng/ đội phó PCCC</t>
+  </si>
+  <si>
+    <t>Trợ cấp sinh hoạt</t>
+  </si>
+  <si>
+    <t>Trợ cấp nuôi con nhỏ dưới 6 tuổi</t>
+  </si>
+  <si>
+    <t>Trợ cấp cho NV nữ</t>
+  </si>
+  <si>
+    <t>Trợ cấp ban ATVSV</t>
+  </si>
+  <si>
+    <t>Trợ cấp tiền cơm</t>
+  </si>
+  <si>
+    <t>Trợ cấp ca đêm</t>
+  </si>
+  <si>
+    <t>Bảo hiểm</t>
+  </si>
+  <si>
+    <t>Thuế TNCN</t>
+  </si>
+  <si>
+    <t>Tạm ứng</t>
+  </si>
+  <si>
+    <t>Nghỉ trước thời hạn giấy phép</t>
+  </si>
+  <si>
+    <t>Nghỉ ngang</t>
+  </si>
+  <si>
+    <t>VND 8,000,000</t>
+  </si>
+  <si>
+    <t>26 ngày</t>
+  </si>
+  <si>
+    <t>VND 1,000,000</t>
+  </si>
+  <si>
+    <t>VND 800,000</t>
+  </si>
+  <si>
+    <t>1 ngày</t>
+  </si>
+  <si>
+    <t>VND 335,000</t>
+  </si>
+  <si>
+    <t>0 ngày</t>
+  </si>
+  <si>
+    <t>VND 0</t>
+  </si>
+  <si>
+    <t>VND 660,000</t>
+  </si>
+  <si>
+    <t>VND 600,000</t>
+  </si>
+  <si>
+    <t>VND 400,000</t>
+  </si>
+  <si>
+    <t>VND 350,000</t>
+  </si>
+  <si>
+    <t>VND 200,000</t>
+  </si>
+  <si>
+    <t>24 ngày</t>
+  </si>
+  <si>
+    <t>VND 680,000</t>
+  </si>
+  <si>
+    <t>2 ngày</t>
+  </si>
+  <si>
+    <t>VND 280,000</t>
+  </si>
+  <si>
+    <t>VND 720,000</t>
+  </si>
+  <si>
+    <t>3 ngày</t>
+  </si>
+  <si>
+    <t>VND 700,000</t>
+  </si>
+  <si>
+    <t>VND 615,000</t>
+  </si>
+  <si>
+    <t>VND 461,000</t>
+  </si>
+  <si>
+    <t>5 ngày</t>
+  </si>
+  <si>
+    <t>VND 1,675,000</t>
+  </si>
+  <si>
+    <t>7 ngày</t>
+  </si>
+  <si>
+    <t>VND 269,000</t>
+  </si>
+  <si>
+    <t>VND 840,000</t>
+  </si>
+  <si>
+    <t>9 ngày</t>
+  </si>
+  <si>
+    <t>VND 250,000</t>
+  </si>
+  <si>
+    <t>VND 1,038,000</t>
+  </si>
+  <si>
+    <t>VND 1,500,000</t>
+  </si>
+  <si>
+    <t>10 ngày</t>
+  </si>
+  <si>
+    <t>Maria Johnson</t>
+  </si>
+  <si>
+    <t>Kate OBrien</t>
   </si>
 </sst>
 </file>
@@ -245,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -285,8 +483,14 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -603,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4384F548-7A7C-4771-AC1E-5030EC08539D}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:BA17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -626,9 +830,31 @@
     <col min="17" max="17" width="15.07421875" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21.3046875" style="2" customWidth="1"/>
     <col min="19" max="19" width="16.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.53515625" customWidth="1"/>
+    <col min="22" max="22" width="14.53515625" customWidth="1"/>
+    <col min="23" max="23" width="14.15234375" customWidth="1"/>
+    <col min="24" max="24" width="14" customWidth="1"/>
+    <col min="25" max="26" width="11.84375" customWidth="1"/>
+    <col min="28" max="28" width="13.84375" customWidth="1"/>
+    <col min="30" max="30" width="14" customWidth="1"/>
+    <col min="32" max="32" width="11.921875" customWidth="1"/>
+    <col min="34" max="34" width="11.61328125" customWidth="1"/>
+    <col min="35" max="35" width="14.07421875" customWidth="1"/>
+    <col min="37" max="37" width="11.61328125" customWidth="1"/>
+    <col min="39" max="39" width="13.15234375" customWidth="1"/>
+    <col min="41" max="41" width="13.3828125" customWidth="1"/>
+    <col min="42" max="42" width="12.07421875" customWidth="1"/>
+    <col min="43" max="43" width="12.3046875" customWidth="1"/>
+    <col min="44" max="44" width="12.23046875" customWidth="1"/>
+    <col min="45" max="46" width="11.921875" customWidth="1"/>
+    <col min="47" max="47" width="12.15234375" customWidth="1"/>
+    <col min="48" max="48" width="12.07421875" customWidth="1"/>
+    <col min="49" max="49" width="11.765625" customWidth="1"/>
+    <col min="50" max="50" width="12.07421875" customWidth="1"/>
+    <col min="51" max="51" width="12.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -653,7 +879,7 @@
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -674,66 +900,168 @@
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:53" s="8" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="15" t="s">
+      <c r="R3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="S3" s="17" t="s">
         <v>17</v>
       </c>
+      <c r="T3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB3" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF3" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH3" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI3" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ3" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK3" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL3" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM3" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN3" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP3" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ3" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR3" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS3" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT3" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU3" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX3" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY3" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="BA3" s="15" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -791,13 +1119,115 @@
       <c r="S4" s="5">
         <v>8850769</v>
       </c>
+      <c r="T4" t="s">
+        <v>89</v>
+      </c>
+      <c r="U4" t="s">
+        <v>90</v>
+      </c>
+      <c r="V4" t="s">
+        <v>87</v>
+      </c>
+      <c r="W4" t="s">
+        <v>88</v>
+      </c>
+      <c r="X4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>90</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>24</v>
@@ -850,16 +1280,118 @@
       <c r="S5" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="T5" t="s">
+        <v>87</v>
+      </c>
+      <c r="U5" t="s">
+        <v>99</v>
+      </c>
+      <c r="V5" t="s">
+        <v>89</v>
+      </c>
+      <c r="W5" t="s">
+        <v>90</v>
+      </c>
+      <c r="X5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>111</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>97</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>111</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>90</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D6" s="6">
         <v>45665</v>
@@ -871,46 +1403,208 @@
         <v>6539434276</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="3">
         <v>24</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" s="3">
         <v>1.5</v>
       </c>
       <c r="K6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="Q6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="S6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="S6" s="5" t="s">
-        <v>47</v>
+      <c r="T6" t="s">
+        <v>89</v>
+      </c>
+      <c r="U6" t="s">
+        <v>90</v>
+      </c>
+      <c r="V6" t="s">
+        <v>89</v>
+      </c>
+      <c r="W6" t="s">
+        <v>90</v>
+      </c>
+      <c r="X6" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>114</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>90</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.4">
+      <c r="B8"/>
+      <c r="E8"/>
+      <c r="G8"/>
+      <c r="I8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.4">
+      <c r="B9"/>
+      <c r="E9"/>
+      <c r="G9"/>
+      <c r="I9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.4">
+      <c r="B10"/>
+      <c r="E10"/>
+      <c r="G10"/>
+      <c r="I10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.4">
+      <c r="B11"/>
+      <c r="E11"/>
+      <c r="G11"/>
+      <c r="I11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A14" s="7"/>
       <c r="B14" s="11"/>
       <c r="C14" s="7"/>
@@ -931,7 +1625,7 @@
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A15" s="9"/>
       <c r="B15" s="12"/>
       <c r="C15" s="8"/>
@@ -952,7 +1646,7 @@
       <c r="R15" s="8"/>
       <c r="S15" s="9"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A16" s="9"/>
       <c r="B16" s="12"/>
       <c r="C16" s="8"/>

</xml_diff>

<commit_message>
Big update: fix form + delete all employee
</commit_message>
<xml_diff>
--- a/temp-peyroll-form/Overall-payroll.xlsx
+++ b/temp-peyroll-form/Overall-payroll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Congty\thienphumut\test\thienphumut-hr-backend\temp-peyroll-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B495A0DD-5E7E-47BA-BC5E-9C35EE0C64B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0AF750-7C3B-418A-90C8-D9D6D34512C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10910" yWindow="-110" windowWidth="11020" windowHeight="18700" xr2:uid="{D457F286-B932-415A-9CBA-56FD1E6E92B6}"/>
+    <workbookView xWindow="-19290" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{D457F286-B932-415A-9CBA-56FD1E6E92B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
   <si>
     <t>Mã NV</t>
   </si>
@@ -96,84 +96,6 @@
     <t>10/2025</t>
   </si>
   <si>
-    <t>VND 40,000</t>
-  </si>
-  <si>
-    <t>Kế toán</t>
-  </si>
-  <si>
-    <t>15/09/2025</t>
-  </si>
-  <si>
-    <t>VND 7,000,000</t>
-  </si>
-  <si>
-    <t>VND 9,000,000</t>
-  </si>
-  <si>
-    <t>VND 7,800,000</t>
-  </si>
-  <si>
-    <t>VND 202,500</t>
-  </si>
-  <si>
-    <t>VND 450,000</t>
-  </si>
-  <si>
-    <t>VND 900,000</t>
-  </si>
-  <si>
-    <t>VND 300,000</t>
-  </si>
-  <si>
-    <t>VND 9,652,500</t>
-  </si>
-  <si>
-    <t>VND 756,000</t>
-  </si>
-  <si>
-    <t>VND 796,000</t>
-  </si>
-  <si>
-    <t>VND 8,856,500</t>
-  </si>
-  <si>
-    <t>Nhân sự</t>
-  </si>
-  <si>
-    <t>VND 11,500,000</t>
-  </si>
-  <si>
-    <t>VND 8,846,154</t>
-  </si>
-  <si>
-    <t>VND 99,038</t>
-  </si>
-  <si>
-    <t>VND 500,000</t>
-  </si>
-  <si>
-    <t>VND 1,200,000</t>
-  </si>
-  <si>
-    <t>VND 11,145,192</t>
-  </si>
-  <si>
-    <t>VND 966,000</t>
-  </si>
-  <si>
-    <t>VND 1,006,000</t>
-  </si>
-  <si>
-    <t>VND 10,139,192</t>
-  </si>
-  <si>
-    <t>01116</t>
-  </si>
-  <si>
-    <t>01117</t>
-  </si>
-  <si>
     <t>Số ngày lễ</t>
   </si>
   <si>
@@ -276,106 +198,43 @@
     <t>Nghỉ ngang</t>
   </si>
   <si>
-    <t>VND 8,000,000</t>
-  </si>
-  <si>
     <t>26 ngày</t>
   </si>
   <si>
-    <t>VND 1,000,000</t>
-  </si>
-  <si>
-    <t>VND 800,000</t>
-  </si>
-  <si>
     <t>1 ngày</t>
   </si>
   <si>
-    <t>VND 335,000</t>
-  </si>
-  <si>
     <t>0 ngày</t>
   </si>
   <si>
     <t>VND 0</t>
   </si>
   <si>
-    <t>VND 660,000</t>
-  </si>
-  <si>
-    <t>VND 600,000</t>
-  </si>
-  <si>
-    <t>VND 400,000</t>
-  </si>
-  <si>
-    <t>VND 350,000</t>
-  </si>
-  <si>
-    <t>VND 200,000</t>
-  </si>
-  <si>
-    <t>24 ngày</t>
-  </si>
-  <si>
-    <t>VND 680,000</t>
-  </si>
-  <si>
     <t>2 ngày</t>
   </si>
   <si>
-    <t>VND 280,000</t>
-  </si>
-  <si>
-    <t>VND 720,000</t>
-  </si>
-  <si>
-    <t>3 ngày</t>
-  </si>
-  <si>
-    <t>VND 700,000</t>
-  </si>
-  <si>
-    <t>VND 615,000</t>
-  </si>
-  <si>
-    <t>VND 461,000</t>
-  </si>
-  <si>
     <t>5 ngày</t>
   </si>
   <si>
-    <t>VND 1,675,000</t>
-  </si>
-  <si>
     <t>7 ngày</t>
   </si>
   <si>
-    <t>VND 269,000</t>
-  </si>
-  <si>
-    <t>VND 840,000</t>
-  </si>
-  <si>
-    <t>9 ngày</t>
-  </si>
-  <si>
-    <t>VND 250,000</t>
-  </si>
-  <si>
-    <t>VND 1,038,000</t>
-  </si>
-  <si>
-    <t>VND 1,500,000</t>
-  </si>
-  <si>
-    <t>10 ngày</t>
-  </si>
-  <si>
-    <t>Maria Johnson</t>
-  </si>
-  <si>
-    <t>Kate OBrien</t>
+    <t>Mức lương BHXH</t>
+  </si>
+  <si>
+    <t>Truy thu BHYT</t>
+  </si>
+  <si>
+    <t>25 ngày</t>
+  </si>
+  <si>
+    <t>Điểm PMS</t>
+  </si>
+  <si>
+    <t>Xếp loại PMS</t>
+  </si>
+  <si>
+    <t>Giỏi</t>
   </si>
 </sst>
 </file>
@@ -443,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -491,6 +350,10 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -807,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4384F548-7A7C-4771-AC1E-5030EC08539D}">
-  <dimension ref="A1:BA17"/>
+  <dimension ref="A1:BF17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="AZ1" workbookViewId="0">
+      <selection activeCell="BE6" sqref="BE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -852,9 +715,13 @@
     <col min="49" max="49" width="11.765625" customWidth="1"/>
     <col min="50" max="50" width="12.07421875" customWidth="1"/>
     <col min="51" max="51" width="12.23046875" customWidth="1"/>
+    <col min="52" max="52" width="12.765625" customWidth="1"/>
+    <col min="53" max="53" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.07421875" customWidth="1"/>
+    <col min="55" max="55" width="11.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -879,7 +746,7 @@
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -900,7 +767,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
     </row>
-    <row r="3" spans="1:53" s="8" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:58" s="8" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
@@ -959,109 +826,121 @@
         <v>17</v>
       </c>
       <c r="T3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO3" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR3" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="AS3" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT3" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="AU3" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="AV3" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="W3" s="15" t="s">
+      <c r="AW3" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="AX3" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="AY3" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="Z3" s="15" t="s">
+      <c r="AZ3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="AA3" s="15" t="s">
+      <c r="BA3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="AB3" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC3" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD3" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE3" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF3" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG3" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH3" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI3" s="15" t="s">
+      <c r="BB3" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="AJ3" s="15" t="s">
+      <c r="BC3" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="AK3" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL3" s="15" t="s">
+      <c r="BD3" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="AM3" s="15" t="s">
+      <c r="BE3" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="AN3" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO3" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP3" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ3" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="AR3" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS3" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT3" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="AU3" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AV3" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="AW3" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="AX3" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="AY3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="AZ3" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="BA3" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1083,14 +962,14 @@
       <c r="G4" s="5">
         <v>10000000</v>
       </c>
-      <c r="H4" s="3">
-        <v>25</v>
+      <c r="H4" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="I4" s="5">
         <v>7692308</v>
       </c>
-      <c r="J4" s="3">
-        <v>2</v>
+      <c r="J4" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="K4" s="5">
         <v>115385</v>
@@ -1120,431 +999,155 @@
         <v>8850769</v>
       </c>
       <c r="T4" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="U4" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="V4" t="s">
-        <v>87</v>
-      </c>
-      <c r="W4" t="s">
-        <v>88</v>
-      </c>
-      <c r="X4" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>30</v>
+        <v>58</v>
+      </c>
+      <c r="W4" s="5">
+        <v>335000</v>
+      </c>
+      <c r="X4" s="5">
+        <v>800000</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>400000</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>450000</v>
       </c>
       <c r="AA4" t="s">
-        <v>98</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>103</v>
+        <v>61</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>615000</v>
       </c>
       <c r="AC4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>104</v>
+        <v>58</v>
+      </c>
+      <c r="AD4" s="5">
+        <v>461000</v>
       </c>
       <c r="AE4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>41</v>
+        <v>57</v>
+      </c>
+      <c r="AF4" s="5">
+        <v>500000</v>
       </c>
       <c r="AG4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>85</v>
+        <v>59</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>1000000</v>
       </c>
       <c r="AJ4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>90</v>
+        <v>59</v>
+      </c>
+      <c r="AK4" s="5">
+        <v>0</v>
       </c>
       <c r="AL4" t="s">
-        <v>105</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>106</v>
+        <v>62</v>
+      </c>
+      <c r="AM4" s="5">
+        <v>1675000</v>
       </c>
       <c r="AN4" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>86</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>90</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="3">
-        <v>6530734221</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="3">
-        <v>26</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="3">
-        <v>3</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="T5" t="s">
-        <v>87</v>
-      </c>
-      <c r="U5" t="s">
-        <v>99</v>
-      </c>
-      <c r="V5" t="s">
-        <v>89</v>
-      </c>
-      <c r="W5" t="s">
-        <v>90</v>
-      </c>
-      <c r="X5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>101</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>109</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>111</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>95</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>95</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>97</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>111</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>90</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="6">
-        <v>45665</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="3">
-        <v>6539434276</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="3">
-        <v>24</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="T6" t="s">
-        <v>89</v>
-      </c>
-      <c r="U6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V6" t="s">
-        <v>89</v>
-      </c>
-      <c r="W6" t="s">
-        <v>90</v>
-      </c>
-      <c r="X6" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>112</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>112</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>113</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>98</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>100</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>114</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>93</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>100</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>92</v>
-      </c>
-      <c r="AY6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AZ6" t="s">
-        <v>90</v>
-      </c>
-      <c r="BA6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.4">
+        <v>63</v>
+      </c>
+      <c r="AO4" s="5">
+        <v>8000000</v>
+      </c>
+      <c r="AP4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="5">
+        <v>300000</v>
+      </c>
+      <c r="AR4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="5">
+        <v>200000</v>
+      </c>
+      <c r="AU4" s="5">
+        <v>660000</v>
+      </c>
+      <c r="AV4" s="5">
+        <v>350000</v>
+      </c>
+      <c r="AW4" s="5">
+        <v>800000</v>
+      </c>
+      <c r="AX4" s="5">
+        <v>450000</v>
+      </c>
+      <c r="AY4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="5">
+        <v>111000</v>
+      </c>
+      <c r="BA4" s="5">
+        <v>23000</v>
+      </c>
+      <c r="BB4" s="5">
+        <v>360000</v>
+      </c>
+      <c r="BC4" s="5">
+        <v>840000</v>
+      </c>
+      <c r="BD4" s="19">
+        <v>9</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>69</v>
+      </c>
+      <c r="BF4" s="5"/>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.4">
+      <c r="B5"/>
+      <c r="E5"/>
+      <c r="G5"/>
+      <c r="I5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+    </row>
+    <row r="6" spans="1:58" x14ac:dyDescent="0.4">
+      <c r="B6"/>
+      <c r="E6"/>
+      <c r="G6"/>
+      <c r="I6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.4">
+      <c r="AC7" s="18"/>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.4">
       <c r="B8"/>
       <c r="E8"/>
       <c r="G8"/>
@@ -1559,7 +1162,7 @@
       <c r="R8"/>
       <c r="S8"/>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.4">
       <c r="B9"/>
       <c r="E9"/>
       <c r="G9"/>
@@ -1574,7 +1177,7 @@
       <c r="R9"/>
       <c r="S9"/>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.4">
       <c r="B10"/>
       <c r="E10"/>
       <c r="G10"/>
@@ -1589,7 +1192,7 @@
       <c r="R10"/>
       <c r="S10"/>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.4">
       <c r="B11"/>
       <c r="E11"/>
       <c r="G11"/>
@@ -1604,7 +1207,7 @@
       <c r="R11"/>
       <c r="S11"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A14" s="7"/>
       <c r="B14" s="11"/>
       <c r="C14" s="7"/>
@@ -1625,7 +1228,7 @@
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A15" s="9"/>
       <c r="B15" s="12"/>
       <c r="C15" s="8"/>
@@ -1646,7 +1249,7 @@
       <c r="R15" s="8"/>
       <c r="S15" s="9"/>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A16" s="9"/>
       <c r="B16" s="12"/>
       <c r="C16" s="8"/>

</xml_diff>